<commit_message>
alterando informações da planilha de clientes
</commit_message>
<xml_diff>
--- a/clientes.xlsx
+++ b/clientes.xlsx
@@ -550,7 +550,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="4">
-        <v>5561993145186</v>
+        <v>0</v>
       </c>
       <c r="C10" s="5">
         <v>25568.875520833335</v>
@@ -561,7 +561,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="4">
-        <v>5561993145186</v>
+        <v>0</v>
       </c>
       <c r="C11" s="5">
         <v>25568.875520833335</v>
@@ -572,7 +572,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="4">
-        <v>5561993145186</v>
+        <v>0</v>
       </c>
       <c r="C12" s="5">
         <v>25568.875520833335</v>

</xml_diff>